<commit_message>
fix: extração dos nomes dos vendedores da amazon e mercado livre
</commit_message>
<xml_diff>
--- a/data/raw_data/scraping_data.xlsx
+++ b/data/raw_data/scraping_data.xlsx
@@ -496,12 +496,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['1.049', '00', 0.01049]</t>
+          <t>Shop Favs</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-03-30 17:32:36</t>
+          <t>2025-03-30 18:20:06</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -536,12 +536,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['1.004', '27', 0.0100427]</t>
+          <t>Amazon.com.br</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-03-30 17:32:37</t>
+          <t>2025-03-30 18:20:07</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -572,12 +572,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[4299, 0, 42.99]</t>
+          <t>Mercado Livre Eletronicos</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-03-30 17:32:37</t>
+          <t>2025-03-30 18:20:07</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -608,12 +608,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[5158, 0, 51.58]</t>
+          <t>SOMA3046530</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-03-30 17:32:38</t>
+          <t>2025-03-30 18:20:08</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">

</xml_diff>

<commit_message>
fix: preço realizado pelo scrape do amazon e mercado livre
</commit_message>
<xml_diff>
--- a/data/raw_data/scraping_data.xlsx
+++ b/data/raw_data/scraping_data.xlsx
@@ -481,18 +481,14 @@
           <t>Monitor Gamer LG UltraGear 24” 24GS60F-B IPS Full HD 180Hz 1ms (GtG) NVIDIA® G-SYNC® AMD FreeSync™ HDR10 sRGB 99% HDMI DisplayPort</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1.049</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>00</t>
-        </is>
+      <c r="B2" t="n">
+        <v>1049</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01049</v>
+        <v>1049</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -501,7 +497,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-03-30 18:20:06</t>
+          <t>2025-03-30 18:57:10</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -521,18 +517,14 @@
           <t>Monitor Gamer AOC HERO QUAD 27" 155Hz QHD 1440p 1ms AMD FreeSync Q27G2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1.004</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
+      <c r="B3" t="n">
+        <v>1004</v>
+      </c>
+      <c r="C3" t="n">
+        <v>27</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0100427</v>
+        <v>1004.27</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -541,7 +533,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-03-30 18:20:07</t>
+          <t>2025-03-30 18:57:10</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -568,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>42.99</v>
+        <v>4299</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -577,7 +569,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-03-30 18:20:07</t>
+          <t>2025-03-30 18:57:11</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -604,7 +596,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>51.58</v>
+        <v>5158</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -613,7 +605,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-03-30 18:20:08</t>
+          <t>2025-03-30 18:57:12</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">

</xml_diff>